<commit_message>
changed urls and views in profiles
</commit_message>
<xml_diff>
--- a/urls.xlsx
+++ b/urls.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\КПІ\3 курс 2 семестр\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Іванка\3 курс\2 семестр\Python\Learniverse\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECCFDB2B-D944-4264-8CBB-275B1A577B9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Аркуш1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="57">
   <si>
     <t xml:space="preserve">Domain name: </t>
   </si>
@@ -57,12 +58,6 @@
     <t>/profile/login</t>
   </si>
   <si>
-    <t>/student/profile</t>
-  </si>
-  <si>
-    <t>/student/courses</t>
-  </si>
-  <si>
     <t>/about</t>
   </si>
   <si>
@@ -78,24 +73,6 @@
     <t>/courses/{id}/module/{id_module}/test/{id_test}</t>
   </si>
   <si>
-    <t>student/wishlist</t>
-  </si>
-  <si>
-    <t>/teacher/profile</t>
-  </si>
-  <si>
-    <t>/teacher/courses</t>
-  </si>
-  <si>
-    <t>/teacher/course/{id_course}</t>
-  </si>
-  <si>
-    <t>/teacher/add_course</t>
-  </si>
-  <si>
-    <t>teacher/delete_course/{id_course}</t>
-  </si>
-  <si>
     <t xml:space="preserve">Method: </t>
   </si>
   <si>
@@ -189,12 +166,6 @@
     <t>Wish list page</t>
   </si>
   <si>
-    <t>Profile teacher page</t>
-  </si>
-  <si>
-    <t>Courses for teacher</t>
-  </si>
-  <si>
     <t>Course page for teacher</t>
   </si>
   <si>
@@ -202,13 +173,31 @@
   </si>
   <si>
     <t>Delete course</t>
+  </si>
+  <si>
+    <t>/profile</t>
+  </si>
+  <si>
+    <t>/profile/courses</t>
+  </si>
+  <si>
+    <t>profile/wishlist</t>
+  </si>
+  <si>
+    <t>/profile/course/{id_course}</t>
+  </si>
+  <si>
+    <t>/profiles/add_course</t>
+  </si>
+  <si>
+    <t>/profiles/delete_course/{id_course}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -275,13 +264,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -493,17 +482,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:W7"/>
+  <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="U12" sqref="U12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
     <col min="2" max="2" width="16.21875" customWidth="1"/>
@@ -517,14 +506,13 @@
     <col min="15" max="15" width="36.6640625" customWidth="1"/>
     <col min="16" max="16" width="38.77734375" customWidth="1"/>
     <col min="17" max="17" width="17.109375" customWidth="1"/>
-    <col min="18" max="19" width="16.33203125" customWidth="1"/>
-    <col min="20" max="20" width="23.6640625" customWidth="1"/>
-    <col min="21" max="21" width="17.77734375" customWidth="1"/>
-    <col min="22" max="22" width="18" customWidth="1"/>
-    <col min="23" max="23" width="29.88671875" customWidth="1"/>
+    <col min="18" max="18" width="23.6640625" customWidth="1"/>
+    <col min="19" max="19" width="17.77734375" customWidth="1"/>
+    <col min="20" max="20" width="18" customWidth="1"/>
+    <col min="21" max="21" width="29.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -588,14 +576,8 @@
       <c r="U1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="V1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>1</v>
-      </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -659,14 +641,8 @@
       <c r="U2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="V2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -692,359 +668,327 @@
         <v>11</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="P3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q3" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="H4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="C5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="F5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="W3" s="1" t="s">
-        <v>24</v>
+      <c r="M5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
-      <c r="A4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>26</v>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
-      <c r="A5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="1" t="s">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M5" s="1" t="s">
+      <c r="C7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="P5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="T5" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="U5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23">
-      <c r="A6" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="H7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="V6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="W6" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23">
-      <c r="A7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="K7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="O7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="P7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="Q7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="R7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="S7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="T7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="U7" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="V7" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="W7" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1"/>
-    <hyperlink ref="C1" r:id="rId2"/>
-    <hyperlink ref="D1" r:id="rId3"/>
-    <hyperlink ref="E1" r:id="rId4"/>
-    <hyperlink ref="F1" r:id="rId5"/>
-    <hyperlink ref="G1" r:id="rId6"/>
-    <hyperlink ref="H1" r:id="rId7"/>
-    <hyperlink ref="I1" r:id="rId8"/>
-    <hyperlink ref="J1" r:id="rId9"/>
-    <hyperlink ref="K1" r:id="rId10"/>
-    <hyperlink ref="L1" r:id="rId11"/>
-    <hyperlink ref="M1" r:id="rId12"/>
-    <hyperlink ref="N1" r:id="rId13"/>
-    <hyperlink ref="O1" r:id="rId14"/>
-    <hyperlink ref="P1" r:id="rId15"/>
-    <hyperlink ref="Q1" r:id="rId16"/>
-    <hyperlink ref="R1" r:id="rId17"/>
-    <hyperlink ref="S1" r:id="rId18"/>
-    <hyperlink ref="T1" r:id="rId19"/>
-    <hyperlink ref="U1" r:id="rId20"/>
-    <hyperlink ref="V1" r:id="rId21"/>
-    <hyperlink ref="W1" r:id="rId22"/>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C1" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D1" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E1" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="F1" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G1" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="H1" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="I1" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="J1" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="K1" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="L1" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="M1" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="N1" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="O1" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="P1" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="Q1" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="R1" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="S1" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="T1" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="U1" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>